<commit_message>
Continued HMC, explored weather.
</commit_message>
<xml_diff>
--- a/data/ratings.xlsx
+++ b/data/ratings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ML\WineML\GrandCruClassifier\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3639A2DE-85A5-403B-8347-8E1329CEFB4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F726A80C-8D22-4C95-9A48-BFB9CBE61E2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="29">
   <si>
     <t>Vintage</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Petrus Pomerol</t>
+  </si>
+  <si>
+    <t>Château Pavie</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G277"/>
+  <dimension ref="A1:G302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="D278" sqref="D278"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="A278" sqref="A278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6829,6 +6832,581 @@
         <v>43556</v>
       </c>
       <c r="G277" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7">
+      <c r="A278" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B278" t="s">
+        <v>23</v>
+      </c>
+      <c r="C278" s="1">
+        <v>1994</v>
+      </c>
+      <c r="D278">
+        <v>85</v>
+      </c>
+      <c r="E278">
+        <v>87</v>
+      </c>
+      <c r="F278" s="2">
+        <v>34790</v>
+      </c>
+      <c r="G278" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7">
+      <c r="A279" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B279" t="s">
+        <v>23</v>
+      </c>
+      <c r="C279" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D279">
+        <v>85</v>
+      </c>
+      <c r="E279">
+        <v>87</v>
+      </c>
+      <c r="F279" s="2">
+        <v>35156</v>
+      </c>
+      <c r="G279" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B280" t="s">
+        <v>23</v>
+      </c>
+      <c r="C280" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D280">
+        <v>85</v>
+      </c>
+      <c r="E280">
+        <v>87</v>
+      </c>
+      <c r="F280" s="2">
+        <v>35796</v>
+      </c>
+      <c r="G280" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7">
+      <c r="A281" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B281" t="s">
+        <v>23</v>
+      </c>
+      <c r="C281" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D281">
+        <v>83</v>
+      </c>
+      <c r="E281">
+        <v>85</v>
+      </c>
+      <c r="F281" s="2">
+        <v>35886</v>
+      </c>
+      <c r="G281" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7">
+      <c r="A282" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B282" t="s">
+        <v>23</v>
+      </c>
+      <c r="C282" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D282">
+        <v>91</v>
+      </c>
+      <c r="E282">
+        <v>93</v>
+      </c>
+      <c r="F282" s="2">
+        <v>36251</v>
+      </c>
+      <c r="G282" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7">
+      <c r="A283" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B283" t="s">
+        <v>23</v>
+      </c>
+      <c r="C283" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D283">
+        <v>92</v>
+      </c>
+      <c r="E283">
+        <v>96</v>
+      </c>
+      <c r="F283" s="2">
+        <v>36617</v>
+      </c>
+      <c r="G283" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7">
+      <c r="A284" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B284" t="s">
+        <v>23</v>
+      </c>
+      <c r="C284" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D284">
+        <v>95</v>
+      </c>
+      <c r="E284">
+        <v>96</v>
+      </c>
+      <c r="F284" s="2">
+        <v>36982</v>
+      </c>
+      <c r="G284" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7">
+      <c r="A285" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B285" t="s">
+        <v>23</v>
+      </c>
+      <c r="C285" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D285">
+        <v>94</v>
+      </c>
+      <c r="E285">
+        <v>96</v>
+      </c>
+      <c r="F285" s="2">
+        <v>37347</v>
+      </c>
+      <c r="G285" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7">
+      <c r="A286" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B286" t="s">
+        <v>23</v>
+      </c>
+      <c r="C286" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D286">
+        <v>92</v>
+      </c>
+      <c r="E286">
+        <v>95</v>
+      </c>
+      <c r="F286" s="2">
+        <v>37895</v>
+      </c>
+      <c r="G286" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7">
+      <c r="A287" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B287" t="s">
+        <v>23</v>
+      </c>
+      <c r="C287" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D287">
+        <v>96</v>
+      </c>
+      <c r="E287">
+        <v>100</v>
+      </c>
+      <c r="F287" s="2">
+        <v>38078</v>
+      </c>
+      <c r="G287" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7">
+      <c r="A288" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B288" t="s">
+        <v>23</v>
+      </c>
+      <c r="C288" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D288">
+        <v>95</v>
+      </c>
+      <c r="E288">
+        <v>97</v>
+      </c>
+      <c r="F288" s="2">
+        <v>38443</v>
+      </c>
+      <c r="G288" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7">
+      <c r="A289" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B289" t="s">
+        <v>23</v>
+      </c>
+      <c r="C289" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D289">
+        <v>98</v>
+      </c>
+      <c r="E289">
+        <v>100</v>
+      </c>
+      <c r="F289" s="2">
+        <v>38808</v>
+      </c>
+      <c r="G289" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7">
+      <c r="A290" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B290" t="s">
+        <v>23</v>
+      </c>
+      <c r="C290" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D290">
+        <v>96</v>
+      </c>
+      <c r="E290">
+        <v>98</v>
+      </c>
+      <c r="F290" s="2">
+        <v>39173</v>
+      </c>
+      <c r="G290" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7">
+      <c r="A291" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B291" t="s">
+        <v>23</v>
+      </c>
+      <c r="C291" s="1">
+        <v>2007</v>
+      </c>
+      <c r="D291">
+        <v>93</v>
+      </c>
+      <c r="E291">
+        <v>95</v>
+      </c>
+      <c r="F291" s="2">
+        <v>39539</v>
+      </c>
+      <c r="G291" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7">
+      <c r="A292" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B292" t="s">
+        <v>23</v>
+      </c>
+      <c r="C292" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D292">
+        <v>96</v>
+      </c>
+      <c r="E292">
+        <v>98</v>
+      </c>
+      <c r="F292" s="2">
+        <v>39904</v>
+      </c>
+      <c r="G292" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7">
+      <c r="A293" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B293" t="s">
+        <v>23</v>
+      </c>
+      <c r="C293" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D293">
+        <v>96</v>
+      </c>
+      <c r="E293">
+        <v>100</v>
+      </c>
+      <c r="F293" s="2">
+        <v>40269</v>
+      </c>
+      <c r="G293" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7">
+      <c r="A294" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B294" t="s">
+        <v>23</v>
+      </c>
+      <c r="C294" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D294">
+        <v>95</v>
+      </c>
+      <c r="E294">
+        <v>98</v>
+      </c>
+      <c r="F294" s="2">
+        <v>40664</v>
+      </c>
+      <c r="G294" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7">
+      <c r="A295" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B295" t="s">
+        <v>23</v>
+      </c>
+      <c r="C295" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D295">
+        <v>93</v>
+      </c>
+      <c r="E295">
+        <v>95</v>
+      </c>
+      <c r="F295" s="2">
+        <v>41000</v>
+      </c>
+      <c r="G295" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7">
+      <c r="A296" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B296" t="s">
+        <v>23</v>
+      </c>
+      <c r="C296" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D296">
+        <v>94</v>
+      </c>
+      <c r="E296">
+        <v>96</v>
+      </c>
+      <c r="F296" s="2">
+        <v>41365</v>
+      </c>
+      <c r="G296" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7">
+      <c r="A297" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B297" t="s">
+        <v>23</v>
+      </c>
+      <c r="C297" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D297">
+        <v>92</v>
+      </c>
+      <c r="E297">
+        <v>94</v>
+      </c>
+      <c r="F297" s="2">
+        <v>41852</v>
+      </c>
+      <c r="G297" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7">
+      <c r="A298" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B298" t="s">
+        <v>23</v>
+      </c>
+      <c r="C298" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D298">
+        <v>94</v>
+      </c>
+      <c r="E298">
+        <v>96</v>
+      </c>
+      <c r="F298" s="2">
+        <v>42095</v>
+      </c>
+      <c r="G298" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7">
+      <c r="A299" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B299" t="s">
+        <v>23</v>
+      </c>
+      <c r="C299" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D299">
+        <v>96</v>
+      </c>
+      <c r="E299">
+        <v>98</v>
+      </c>
+      <c r="F299" s="2">
+        <v>42461</v>
+      </c>
+      <c r="G299" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7">
+      <c r="A300" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B300" t="s">
+        <v>23</v>
+      </c>
+      <c r="C300" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D300">
+        <v>98</v>
+      </c>
+      <c r="E300">
+        <v>100</v>
+      </c>
+      <c r="F300" s="2">
+        <v>42826</v>
+      </c>
+      <c r="G300" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7">
+      <c r="A301" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B301" t="s">
+        <v>23</v>
+      </c>
+      <c r="C301" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D301">
+        <v>97</v>
+      </c>
+      <c r="E301">
+        <v>99</v>
+      </c>
+      <c r="F301" s="2">
+        <v>43191</v>
+      </c>
+      <c r="G301" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7">
+      <c r="A302" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B302" t="s">
+        <v>23</v>
+      </c>
+      <c r="C302" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D302">
+        <v>97</v>
+      </c>
+      <c r="E302">
+        <v>100</v>
+      </c>
+      <c r="F302" s="2">
+        <v>43556</v>
+      </c>
+      <c r="G302" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more ratings, and may prices.
</commit_message>
<xml_diff>
--- a/data/ratings.xlsx
+++ b/data/ratings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ML\WineML\GrandCruClassifier\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F726A80C-8D22-4C95-9A48-BFB9CBE61E2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CCC07F-34BF-4359-B204-5833DC8A3386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="2592" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First Rating" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="32">
   <si>
     <t>Vintage</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Château Palmer</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Château Lafite Rothschild Pauillac</t>
   </si>
   <si>
@@ -113,6 +110,18 @@
   </si>
   <si>
     <t>Château Pavie</t>
+  </si>
+  <si>
+    <t>Château Léoville Las Cases Saint-Julien</t>
+  </si>
+  <si>
+    <t>Pomerol</t>
+  </si>
+  <si>
+    <t>Saint Emilion</t>
+  </si>
+  <si>
+    <t>Médoc</t>
   </si>
 </sst>
 </file>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G302"/>
+  <dimension ref="A1:G327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="A278" sqref="A278"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="A317" sqref="A317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -489,10 +498,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C2">
         <v>1994</v>
@@ -512,10 +521,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1">
         <v>1995</v>
@@ -535,10 +544,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>1996</v>
@@ -558,10 +567,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>1997</v>
@@ -581,10 +590,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>1998</v>
@@ -604,10 +613,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
         <v>1999</v>
@@ -627,10 +636,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>2000</v>
@@ -650,10 +659,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1">
         <v>2001</v>
@@ -673,10 +682,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>2002</v>
@@ -696,10 +705,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1">
         <v>2003</v>
@@ -719,10 +728,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>2004</v>
@@ -742,10 +751,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1">
         <v>2005</v>
@@ -765,10 +774,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>2006</v>
@@ -788,10 +797,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
         <v>2007</v>
@@ -811,10 +820,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>2008</v>
@@ -834,10 +843,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1">
         <v>2009</v>
@@ -857,10 +866,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>2010</v>
@@ -880,10 +889,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1">
         <v>2011</v>
@@ -903,10 +912,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C20">
         <v>2012</v>
@@ -926,10 +935,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1">
         <v>2013</v>
@@ -949,10 +958,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C22">
         <v>2014</v>
@@ -972,10 +981,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
         <v>2015</v>
@@ -995,10 +1004,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C24">
         <v>2016</v>
@@ -1018,10 +1027,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1">
         <v>2017</v>
@@ -1041,10 +1050,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C26">
         <v>2018</v>
@@ -1064,10 +1073,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C27" s="1">
         <v>2019</v>
@@ -1087,10 +1096,10 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1">
         <v>1994</v>
@@ -1110,10 +1119,10 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>1995</v>
@@ -1133,10 +1142,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1">
         <v>1996</v>
@@ -1156,10 +1165,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>1997</v>
@@ -1179,10 +1188,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1">
         <v>1998</v>
@@ -1202,10 +1211,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C33">
         <v>1999</v>
@@ -1225,10 +1234,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1">
         <v>2000</v>
@@ -1248,10 +1257,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C35">
         <v>2001</v>
@@ -1271,10 +1280,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1">
         <v>2002</v>
@@ -1294,10 +1303,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>2003</v>
@@ -1317,10 +1326,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1">
         <v>2004</v>
@@ -1340,10 +1349,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C39">
         <v>2005</v>
@@ -1363,10 +1372,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1">
         <v>2006</v>
@@ -1386,10 +1395,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C41">
         <v>2007</v>
@@ -1409,10 +1418,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C42" s="1">
         <v>2008</v>
@@ -1432,10 +1441,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C43">
         <v>2009</v>
@@ -1455,10 +1464,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C44" s="1">
         <v>2010</v>
@@ -1478,10 +1487,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C45">
         <v>2011</v>
@@ -1501,10 +1510,10 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C46" s="1">
         <v>2012</v>
@@ -1524,10 +1533,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C47">
         <v>2013</v>
@@ -1547,10 +1556,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C48" s="1">
         <v>2014</v>
@@ -1570,10 +1579,10 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C49">
         <v>2015</v>
@@ -1593,10 +1602,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C50" s="1">
         <v>2016</v>
@@ -1616,10 +1625,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C51">
         <v>2017</v>
@@ -1639,10 +1648,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C52" s="1">
         <v>2018</v>
@@ -1665,7 +1674,7 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C53">
         <v>1994</v>
@@ -1688,7 +1697,7 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C54" s="1">
         <v>1995</v>
@@ -1711,7 +1720,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C55">
         <v>1996</v>
@@ -1734,7 +1743,7 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C56" s="1">
         <v>1997</v>
@@ -1757,7 +1766,7 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C57">
         <v>1998</v>
@@ -1780,7 +1789,7 @@
         <v>4</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1">
         <v>1999</v>
@@ -1803,7 +1812,7 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C59">
         <v>2000</v>
@@ -1826,7 +1835,7 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C60" s="1">
         <v>2001</v>
@@ -1849,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C61">
         <v>2002</v>
@@ -1872,7 +1881,7 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C62" s="1">
         <v>2003</v>
@@ -1895,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C63">
         <v>2004</v>
@@ -1918,7 +1927,7 @@
         <v>4</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C64" s="1">
         <v>2005</v>
@@ -1941,7 +1950,7 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C65">
         <v>2006</v>
@@ -1964,7 +1973,7 @@
         <v>4</v>
       </c>
       <c r="B66" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C66" s="1">
         <v>2007</v>
@@ -1987,7 +1996,7 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C67">
         <v>2008</v>
@@ -2010,7 +2019,7 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C68" s="1">
         <v>2009</v>
@@ -2033,7 +2042,7 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C69">
         <v>2010</v>
@@ -2056,7 +2065,7 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C70" s="1">
         <v>2011</v>
@@ -2079,7 +2088,7 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C71">
         <v>2012</v>
@@ -2102,7 +2111,7 @@
         <v>4</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C72" s="1">
         <v>2013</v>
@@ -2125,7 +2134,7 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C73">
         <v>2014</v>
@@ -2148,7 +2157,7 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C74" s="1">
         <v>2015</v>
@@ -2171,7 +2180,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C75">
         <v>2016</v>
@@ -2194,7 +2203,7 @@
         <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1">
         <v>2017</v>
@@ -2217,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C77">
         <v>2018</v>
@@ -2237,10 +2246,10 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C78" s="1">
         <v>1994</v>
@@ -2260,10 +2269,10 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C79">
         <v>1995</v>
@@ -2283,10 +2292,10 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C80" s="1">
         <v>1996</v>
@@ -2306,10 +2315,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C81">
         <v>1997</v>
@@ -2329,10 +2338,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C82" s="1">
         <v>1998</v>
@@ -2352,10 +2361,10 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C83">
         <v>1999</v>
@@ -2375,10 +2384,10 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C84" s="1">
         <v>2000</v>
@@ -2398,10 +2407,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C85">
         <v>2001</v>
@@ -2421,10 +2430,10 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C86" s="1">
         <v>2002</v>
@@ -2444,10 +2453,10 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C87">
         <v>2003</v>
@@ -2467,10 +2476,10 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C88" s="1">
         <v>2004</v>
@@ -2490,10 +2499,10 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C89">
         <v>2005</v>
@@ -2513,10 +2522,10 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C90" s="1">
         <v>2006</v>
@@ -2536,10 +2545,10 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C91">
         <v>2007</v>
@@ -2559,10 +2568,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C92" s="1">
         <v>2008</v>
@@ -2582,10 +2591,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C93">
         <v>2009</v>
@@ -2605,10 +2614,10 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C94" s="1">
         <v>2010</v>
@@ -2628,10 +2637,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C95">
         <v>2011</v>
@@ -2651,10 +2660,10 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C96" s="1">
         <v>2012</v>
@@ -2674,10 +2683,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C97">
         <v>2013</v>
@@ -2697,10 +2706,10 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C98" s="1">
         <v>2014</v>
@@ -2720,10 +2729,10 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C99">
         <v>2015</v>
@@ -2743,10 +2752,10 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C100" s="1">
         <v>2016</v>
@@ -2766,10 +2775,10 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C101">
         <v>2017</v>
@@ -2789,10 +2798,10 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B102" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C102" s="1">
         <v>2018</v>
@@ -2815,7 +2824,7 @@
         <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C103">
         <v>1994</v>
@@ -2838,7 +2847,7 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C104" s="1">
         <v>1995</v>
@@ -2861,7 +2870,7 @@
         <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C105">
         <v>1996</v>
@@ -2884,7 +2893,7 @@
         <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C106" s="1">
         <v>1997</v>
@@ -2907,7 +2916,7 @@
         <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C107">
         <v>1998</v>
@@ -2930,7 +2939,7 @@
         <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C108" s="1">
         <v>1999</v>
@@ -2953,7 +2962,7 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C109">
         <v>2000</v>
@@ -2976,7 +2985,7 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C110" s="1">
         <v>2001</v>
@@ -2999,7 +3008,7 @@
         <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C111">
         <v>2002</v>
@@ -3022,7 +3031,7 @@
         <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C112" s="1">
         <v>2003</v>
@@ -3045,7 +3054,7 @@
         <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C113">
         <v>2004</v>
@@ -3068,7 +3077,7 @@
         <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C114" s="1">
         <v>2005</v>
@@ -3091,7 +3100,7 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C115">
         <v>2006</v>
@@ -3114,7 +3123,7 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C116" s="1">
         <v>2007</v>
@@ -3137,7 +3146,7 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C117">
         <v>2008</v>
@@ -3160,7 +3169,7 @@
         <v>6</v>
       </c>
       <c r="B118" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C118" s="1">
         <v>2009</v>
@@ -3183,7 +3192,7 @@
         <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C119">
         <v>2010</v>
@@ -3206,7 +3215,7 @@
         <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C120" s="1">
         <v>2011</v>
@@ -3229,7 +3238,7 @@
         <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C121">
         <v>2012</v>
@@ -3252,7 +3261,7 @@
         <v>6</v>
       </c>
       <c r="B122" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C122" s="1">
         <v>2013</v>
@@ -3275,7 +3284,7 @@
         <v>6</v>
       </c>
       <c r="B123" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C123">
         <v>2014</v>
@@ -3298,7 +3307,7 @@
         <v>6</v>
       </c>
       <c r="B124" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C124" s="1">
         <v>2015</v>
@@ -3321,7 +3330,7 @@
         <v>6</v>
       </c>
       <c r="B125" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C125">
         <v>2016</v>
@@ -3344,7 +3353,7 @@
         <v>6</v>
       </c>
       <c r="B126" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C126" s="1">
         <v>2017</v>
@@ -3367,7 +3376,7 @@
         <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C127">
         <v>2018</v>
@@ -3390,7 +3399,7 @@
         <v>7</v>
       </c>
       <c r="B128" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C128" s="1">
         <v>1994</v>
@@ -3413,7 +3422,7 @@
         <v>7</v>
       </c>
       <c r="B129" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C129">
         <v>1995</v>
@@ -3436,7 +3445,7 @@
         <v>7</v>
       </c>
       <c r="B130" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C130" s="1">
         <v>1996</v>
@@ -3459,7 +3468,7 @@
         <v>7</v>
       </c>
       <c r="B131" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C131">
         <v>1997</v>
@@ -3482,7 +3491,7 @@
         <v>7</v>
       </c>
       <c r="B132" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C132" s="1">
         <v>1998</v>
@@ -3505,7 +3514,7 @@
         <v>7</v>
       </c>
       <c r="B133" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C133">
         <v>1999</v>
@@ -3528,7 +3537,7 @@
         <v>7</v>
       </c>
       <c r="B134" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C134" s="1">
         <v>2000</v>
@@ -3551,7 +3560,7 @@
         <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C135">
         <v>2001</v>
@@ -3574,7 +3583,7 @@
         <v>7</v>
       </c>
       <c r="B136" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C136" s="1">
         <v>2002</v>
@@ -3597,7 +3606,7 @@
         <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C137">
         <v>2003</v>
@@ -3620,7 +3629,7 @@
         <v>7</v>
       </c>
       <c r="B138" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C138" s="1">
         <v>2004</v>
@@ -3643,7 +3652,7 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C139">
         <v>2005</v>
@@ -3666,7 +3675,7 @@
         <v>7</v>
       </c>
       <c r="B140" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C140" s="1">
         <v>2006</v>
@@ -3689,7 +3698,7 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C141">
         <v>2007</v>
@@ -3712,7 +3721,7 @@
         <v>7</v>
       </c>
       <c r="B142" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C142" s="1">
         <v>2008</v>
@@ -3735,7 +3744,7 @@
         <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C143">
         <v>2009</v>
@@ -3758,7 +3767,7 @@
         <v>7</v>
       </c>
       <c r="B144" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C144" s="1">
         <v>2010</v>
@@ -3781,7 +3790,7 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C145">
         <v>2011</v>
@@ -3804,7 +3813,7 @@
         <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C146" s="1">
         <v>2012</v>
@@ -3827,7 +3836,7 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C147">
         <v>2013</v>
@@ -3850,7 +3859,7 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C148" s="1">
         <v>2014</v>
@@ -3873,7 +3882,7 @@
         <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C149">
         <v>2015</v>
@@ -3896,7 +3905,7 @@
         <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C150" s="1">
         <v>2016</v>
@@ -3919,7 +3928,7 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C151">
         <v>2017</v>
@@ -3942,7 +3951,7 @@
         <v>7</v>
       </c>
       <c r="B152" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C152" s="1">
         <v>2018</v>
@@ -3965,7 +3974,7 @@
         <v>8</v>
       </c>
       <c r="B153" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C153">
         <v>1994</v>
@@ -3988,7 +3997,7 @@
         <v>8</v>
       </c>
       <c r="B154" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C154" s="1">
         <v>1995</v>
@@ -4011,7 +4020,7 @@
         <v>8</v>
       </c>
       <c r="B155" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C155">
         <v>1996</v>
@@ -4034,7 +4043,7 @@
         <v>8</v>
       </c>
       <c r="B156" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C156" s="1">
         <v>1997</v>
@@ -4057,7 +4066,7 @@
         <v>8</v>
       </c>
       <c r="B157" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C157">
         <v>1998</v>
@@ -4080,7 +4089,7 @@
         <v>8</v>
       </c>
       <c r="B158" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C158" s="1">
         <v>1999</v>
@@ -4103,7 +4112,7 @@
         <v>8</v>
       </c>
       <c r="B159" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C159">
         <v>2000</v>
@@ -4126,7 +4135,7 @@
         <v>8</v>
       </c>
       <c r="B160" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C160" s="1">
         <v>2001</v>
@@ -4149,7 +4158,7 @@
         <v>8</v>
       </c>
       <c r="B161" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C161">
         <v>2002</v>
@@ -4172,7 +4181,7 @@
         <v>8</v>
       </c>
       <c r="B162" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C162" s="1">
         <v>2003</v>
@@ -4195,7 +4204,7 @@
         <v>8</v>
       </c>
       <c r="B163" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C163">
         <v>2004</v>
@@ -4218,7 +4227,7 @@
         <v>8</v>
       </c>
       <c r="B164" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C164" s="1">
         <v>2005</v>
@@ -4241,7 +4250,7 @@
         <v>8</v>
       </c>
       <c r="B165" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C165">
         <v>2006</v>
@@ -4264,7 +4273,7 @@
         <v>8</v>
       </c>
       <c r="B166" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C166" s="1">
         <v>2007</v>
@@ -4287,7 +4296,7 @@
         <v>8</v>
       </c>
       <c r="B167" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C167">
         <v>2008</v>
@@ -4310,7 +4319,7 @@
         <v>8</v>
       </c>
       <c r="B168" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C168" s="1">
         <v>2009</v>
@@ -4333,7 +4342,7 @@
         <v>8</v>
       </c>
       <c r="B169" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C169">
         <v>2010</v>
@@ -4356,7 +4365,7 @@
         <v>8</v>
       </c>
       <c r="B170" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C170" s="1">
         <v>2011</v>
@@ -4379,7 +4388,7 @@
         <v>8</v>
       </c>
       <c r="B171" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C171">
         <v>2012</v>
@@ -4402,7 +4411,7 @@
         <v>8</v>
       </c>
       <c r="B172" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C172" s="1">
         <v>2013</v>
@@ -4425,7 +4434,7 @@
         <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C173">
         <v>2014</v>
@@ -4448,7 +4457,7 @@
         <v>8</v>
       </c>
       <c r="B174" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C174" s="1">
         <v>2015</v>
@@ -4471,7 +4480,7 @@
         <v>8</v>
       </c>
       <c r="B175" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C175">
         <v>2016</v>
@@ -4494,7 +4503,7 @@
         <v>8</v>
       </c>
       <c r="B176" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C176" s="1">
         <v>2017</v>
@@ -4517,7 +4526,7 @@
         <v>8</v>
       </c>
       <c r="B177" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C177">
         <v>2018</v>
@@ -4540,7 +4549,7 @@
         <v>21</v>
       </c>
       <c r="B178" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C178" s="1">
         <v>1994</v>
@@ -4563,7 +4572,7 @@
         <v>21</v>
       </c>
       <c r="B179" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C179" s="1">
         <v>1995</v>
@@ -4586,7 +4595,7 @@
         <v>21</v>
       </c>
       <c r="B180" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C180" s="1">
         <v>1996</v>
@@ -4609,7 +4618,7 @@
         <v>21</v>
       </c>
       <c r="B181" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C181" s="1">
         <v>1997</v>
@@ -4632,7 +4641,7 @@
         <v>21</v>
       </c>
       <c r="B182" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C182" s="1">
         <v>1998</v>
@@ -4655,7 +4664,7 @@
         <v>21</v>
       </c>
       <c r="B183" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C183" s="1">
         <v>1999</v>
@@ -4678,7 +4687,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C184" s="1">
         <v>2000</v>
@@ -4701,7 +4710,7 @@
         <v>21</v>
       </c>
       <c r="B185" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C185" s="1">
         <v>2001</v>
@@ -4724,7 +4733,7 @@
         <v>21</v>
       </c>
       <c r="B186" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C186" s="1">
         <v>2002</v>
@@ -4747,7 +4756,7 @@
         <v>21</v>
       </c>
       <c r="B187" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C187" s="1">
         <v>2003</v>
@@ -4770,7 +4779,7 @@
         <v>21</v>
       </c>
       <c r="B188" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C188" s="1">
         <v>2004</v>
@@ -4793,7 +4802,7 @@
         <v>21</v>
       </c>
       <c r="B189" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C189" s="1">
         <v>2005</v>
@@ -4816,7 +4825,7 @@
         <v>21</v>
       </c>
       <c r="B190" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C190" s="1">
         <v>2006</v>
@@ -4839,7 +4848,7 @@
         <v>21</v>
       </c>
       <c r="B191" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C191" s="1">
         <v>2007</v>
@@ -4862,7 +4871,7 @@
         <v>21</v>
       </c>
       <c r="B192" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C192" s="1">
         <v>2008</v>
@@ -4885,7 +4894,7 @@
         <v>21</v>
       </c>
       <c r="B193" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C193" s="1">
         <v>2009</v>
@@ -4908,7 +4917,7 @@
         <v>21</v>
       </c>
       <c r="B194" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C194" s="1">
         <v>2010</v>
@@ -4931,7 +4940,7 @@
         <v>21</v>
       </c>
       <c r="B195" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C195" s="1">
         <v>2011</v>
@@ -4954,7 +4963,7 @@
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C196" s="1">
         <v>2012</v>
@@ -4977,7 +4986,7 @@
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C197" s="1">
         <v>2013</v>
@@ -5000,7 +5009,7 @@
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C198" s="1">
         <v>2014</v>
@@ -5023,7 +5032,7 @@
         <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C199" s="1">
         <v>2015</v>
@@ -5046,7 +5055,7 @@
         <v>21</v>
       </c>
       <c r="B200" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C200" s="1">
         <v>2016</v>
@@ -5069,7 +5078,7 @@
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C201" s="1">
         <v>2017</v>
@@ -5092,7 +5101,7 @@
         <v>21</v>
       </c>
       <c r="B202" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C202" s="1">
         <v>2018</v>
@@ -5115,7 +5124,7 @@
         <v>20</v>
       </c>
       <c r="B203" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C203" s="1">
         <v>1994</v>
@@ -5138,7 +5147,7 @@
         <v>20</v>
       </c>
       <c r="B204" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C204" s="1">
         <v>1995</v>
@@ -5161,7 +5170,7 @@
         <v>20</v>
       </c>
       <c r="B205" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C205" s="1">
         <v>1996</v>
@@ -5184,7 +5193,7 @@
         <v>20</v>
       </c>
       <c r="B206" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C206" s="1">
         <v>1997</v>
@@ -5207,7 +5216,7 @@
         <v>20</v>
       </c>
       <c r="B207" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C207" s="1">
         <v>1998</v>
@@ -5230,7 +5239,7 @@
         <v>20</v>
       </c>
       <c r="B208" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C208" s="1">
         <v>1999</v>
@@ -5253,7 +5262,7 @@
         <v>20</v>
       </c>
       <c r="B209" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C209" s="1">
         <v>2000</v>
@@ -5276,7 +5285,7 @@
         <v>20</v>
       </c>
       <c r="B210" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C210" s="1">
         <v>2001</v>
@@ -5299,7 +5308,7 @@
         <v>20</v>
       </c>
       <c r="B211" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C211" s="1">
         <v>2002</v>
@@ -5322,7 +5331,7 @@
         <v>20</v>
       </c>
       <c r="B212" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C212" s="1">
         <v>2003</v>
@@ -5345,7 +5354,7 @@
         <v>20</v>
       </c>
       <c r="B213" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C213" s="1">
         <v>2004</v>
@@ -5368,7 +5377,7 @@
         <v>20</v>
       </c>
       <c r="B214" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C214" s="1">
         <v>2005</v>
@@ -5391,7 +5400,7 @@
         <v>20</v>
       </c>
       <c r="B215" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C215" s="1">
         <v>2006</v>
@@ -5414,7 +5423,7 @@
         <v>20</v>
       </c>
       <c r="B216" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C216" s="1">
         <v>2007</v>
@@ -5437,7 +5446,7 @@
         <v>20</v>
       </c>
       <c r="B217" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C217" s="1">
         <v>2008</v>
@@ -5460,7 +5469,7 @@
         <v>20</v>
       </c>
       <c r="B218" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C218" s="1">
         <v>2009</v>
@@ -5483,7 +5492,7 @@
         <v>20</v>
       </c>
       <c r="B219" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C219" s="1">
         <v>2010</v>
@@ -5506,7 +5515,7 @@
         <v>20</v>
       </c>
       <c r="B220" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C220" s="1">
         <v>2011</v>
@@ -5529,7 +5538,7 @@
         <v>20</v>
       </c>
       <c r="B221" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C221" s="1">
         <v>2012</v>
@@ -5552,7 +5561,7 @@
         <v>20</v>
       </c>
       <c r="B222" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C222" s="1">
         <v>2013</v>
@@ -5575,7 +5584,7 @@
         <v>20</v>
       </c>
       <c r="B223" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C223" s="1">
         <v>2014</v>
@@ -5598,7 +5607,7 @@
         <v>20</v>
       </c>
       <c r="B224" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C224" s="1">
         <v>2015</v>
@@ -5621,7 +5630,7 @@
         <v>20</v>
       </c>
       <c r="B225" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C225" s="1">
         <v>2016</v>
@@ -5644,7 +5653,7 @@
         <v>20</v>
       </c>
       <c r="B226" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C226" s="1">
         <v>2017</v>
@@ -5667,7 +5676,7 @@
         <v>20</v>
       </c>
       <c r="B227" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C227" s="1">
         <v>2018</v>
@@ -5690,7 +5699,7 @@
         <v>22</v>
       </c>
       <c r="B228" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C228" s="1">
         <v>1994</v>
@@ -5713,7 +5722,7 @@
         <v>22</v>
       </c>
       <c r="B229" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C229" s="1">
         <v>1995</v>
@@ -5736,7 +5745,7 @@
         <v>22</v>
       </c>
       <c r="B230" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C230" s="1">
         <v>1996</v>
@@ -5759,7 +5768,7 @@
         <v>22</v>
       </c>
       <c r="B231" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C231" s="1">
         <v>1997</v>
@@ -5782,7 +5791,7 @@
         <v>22</v>
       </c>
       <c r="B232" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C232" s="1">
         <v>1998</v>
@@ -5805,7 +5814,7 @@
         <v>22</v>
       </c>
       <c r="B233" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C233" s="1">
         <v>1999</v>
@@ -5828,7 +5837,7 @@
         <v>22</v>
       </c>
       <c r="B234" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C234" s="1">
         <v>2000</v>
@@ -5851,7 +5860,7 @@
         <v>22</v>
       </c>
       <c r="B235" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C235" s="1">
         <v>2001</v>
@@ -5874,7 +5883,7 @@
         <v>22</v>
       </c>
       <c r="B236" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C236" s="1">
         <v>2002</v>
@@ -5897,7 +5906,7 @@
         <v>22</v>
       </c>
       <c r="B237" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C237" s="1">
         <v>2003</v>
@@ -5920,7 +5929,7 @@
         <v>22</v>
       </c>
       <c r="B238" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C238" s="1">
         <v>2004</v>
@@ -5943,7 +5952,7 @@
         <v>22</v>
       </c>
       <c r="B239" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C239" s="1">
         <v>2005</v>
@@ -5966,7 +5975,7 @@
         <v>22</v>
       </c>
       <c r="B240" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C240" s="1">
         <v>2006</v>
@@ -5989,7 +5998,7 @@
         <v>22</v>
       </c>
       <c r="B241" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C241" s="1">
         <v>2007</v>
@@ -6012,7 +6021,7 @@
         <v>22</v>
       </c>
       <c r="B242" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C242" s="1">
         <v>2008</v>
@@ -6035,7 +6044,7 @@
         <v>22</v>
       </c>
       <c r="B243" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C243" s="1">
         <v>2009</v>
@@ -6058,7 +6067,7 @@
         <v>22</v>
       </c>
       <c r="B244" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C244" s="1">
         <v>2010</v>
@@ -6081,7 +6090,7 @@
         <v>22</v>
       </c>
       <c r="B245" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C245" s="1">
         <v>2011</v>
@@ -6104,7 +6113,7 @@
         <v>22</v>
       </c>
       <c r="B246" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C246" s="1">
         <v>2012</v>
@@ -6127,7 +6136,7 @@
         <v>22</v>
       </c>
       <c r="B247" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C247" s="1">
         <v>2013</v>
@@ -6150,7 +6159,7 @@
         <v>22</v>
       </c>
       <c r="B248" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C248" s="1">
         <v>2014</v>
@@ -6173,7 +6182,7 @@
         <v>22</v>
       </c>
       <c r="B249" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C249" s="1">
         <v>2015</v>
@@ -6196,7 +6205,7 @@
         <v>22</v>
       </c>
       <c r="B250" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C250" s="1">
         <v>2016</v>
@@ -6219,7 +6228,7 @@
         <v>22</v>
       </c>
       <c r="B251" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C251" s="1">
         <v>2017</v>
@@ -6242,7 +6251,7 @@
         <v>22</v>
       </c>
       <c r="B252" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C252" s="1">
         <v>2018</v>
@@ -6262,10 +6271,10 @@
     </row>
     <row r="253" spans="1:7">
       <c r="A253" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B253" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C253" s="1">
         <v>1994</v>
@@ -6285,10 +6294,10 @@
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B254" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C254" s="1">
         <v>1995</v>
@@ -6308,10 +6317,10 @@
     </row>
     <row r="255" spans="1:7">
       <c r="A255" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B255" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C255" s="1">
         <v>1996</v>
@@ -6331,10 +6340,10 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B256" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C256" s="1">
         <v>1997</v>
@@ -6354,10 +6363,10 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B257" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C257" s="1">
         <v>1998</v>
@@ -6377,10 +6386,10 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B258" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C258" s="1">
         <v>1999</v>
@@ -6400,10 +6409,10 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B259" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C259" s="1">
         <v>2000</v>
@@ -6423,10 +6432,10 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B260" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C260" s="1">
         <v>2001</v>
@@ -6446,10 +6455,10 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B261" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C261" s="1">
         <v>2002</v>
@@ -6469,10 +6478,10 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B262" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C262" s="1">
         <v>2003</v>
@@ -6492,10 +6501,10 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B263" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C263" s="1">
         <v>2004</v>
@@ -6515,10 +6524,10 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B264" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C264" s="1">
         <v>2005</v>
@@ -6538,10 +6547,10 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B265" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C265" s="1">
         <v>2006</v>
@@ -6561,10 +6570,10 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B266" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C266" s="1">
         <v>2007</v>
@@ -6584,10 +6593,10 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B267" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C267" s="1">
         <v>2008</v>
@@ -6607,10 +6616,10 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B268" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C268" s="1">
         <v>2009</v>
@@ -6630,10 +6639,10 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B269" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C269" s="1">
         <v>2010</v>
@@ -6653,10 +6662,10 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B270" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C270" s="1">
         <v>2011</v>
@@ -6676,10 +6685,10 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B271" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C271" s="1">
         <v>2012</v>
@@ -6699,10 +6708,10 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B272" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C272" s="1">
         <v>2013</v>
@@ -6722,10 +6731,10 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B273" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C273" s="1">
         <v>2014</v>
@@ -6745,10 +6754,10 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B274" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C274" s="1">
         <v>2015</v>
@@ -6768,10 +6777,10 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B275" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C275" s="1">
         <v>2016</v>
@@ -6791,10 +6800,10 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B276" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C276" s="1">
         <v>2017</v>
@@ -6814,10 +6823,10 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B277" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C277" s="1">
         <v>2018</v>
@@ -6837,10 +6846,10 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B278" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C278" s="1">
         <v>1994</v>
@@ -6860,10 +6869,10 @@
     </row>
     <row r="279" spans="1:7">
       <c r="A279" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B279" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C279" s="1">
         <v>1995</v>
@@ -6883,10 +6892,10 @@
     </row>
     <row r="280" spans="1:7">
       <c r="A280" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B280" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C280" s="1">
         <v>1996</v>
@@ -6906,10 +6915,10 @@
     </row>
     <row r="281" spans="1:7">
       <c r="A281" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B281" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C281" s="1">
         <v>1997</v>
@@ -6929,10 +6938,10 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B282" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C282" s="1">
         <v>1998</v>
@@ -6952,10 +6961,10 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B283" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C283" s="1">
         <v>1999</v>
@@ -6975,10 +6984,10 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B284" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C284" s="1">
         <v>2000</v>
@@ -6998,10 +7007,10 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B285" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C285" s="1">
         <v>2001</v>
@@ -7021,10 +7030,10 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B286" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C286" s="1">
         <v>2002</v>
@@ -7044,10 +7053,10 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B287" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C287" s="1">
         <v>2003</v>
@@ -7067,10 +7076,10 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B288" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C288" s="1">
         <v>2004</v>
@@ -7090,10 +7099,10 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B289" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C289" s="1">
         <v>2005</v>
@@ -7113,10 +7122,10 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B290" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C290" s="1">
         <v>2006</v>
@@ -7136,10 +7145,10 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B291" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C291" s="1">
         <v>2007</v>
@@ -7159,10 +7168,10 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B292" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C292" s="1">
         <v>2008</v>
@@ -7182,10 +7191,10 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B293" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C293" s="1">
         <v>2009</v>
@@ -7205,10 +7214,10 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B294" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C294" s="1">
         <v>2010</v>
@@ -7228,10 +7237,10 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B295" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C295" s="1">
         <v>2011</v>
@@ -7251,10 +7260,10 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B296" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C296" s="1">
         <v>2012</v>
@@ -7274,10 +7283,10 @@
     </row>
     <row r="297" spans="1:7">
       <c r="A297" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B297" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C297" s="1">
         <v>2013</v>
@@ -7297,10 +7306,10 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B298" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C298" s="1">
         <v>2014</v>
@@ -7320,10 +7329,10 @@
     </row>
     <row r="299" spans="1:7">
       <c r="A299" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B299" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C299" s="1">
         <v>2015</v>
@@ -7343,10 +7352,10 @@
     </row>
     <row r="300" spans="1:7">
       <c r="A300" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B300" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C300" s="1">
         <v>2016</v>
@@ -7366,10 +7375,10 @@
     </row>
     <row r="301" spans="1:7">
       <c r="A301" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B301" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C301" s="1">
         <v>2017</v>
@@ -7389,10 +7398,10 @@
     </row>
     <row r="302" spans="1:7">
       <c r="A302" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B302" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C302" s="1">
         <v>2018</v>
@@ -7407,6 +7416,581 @@
         <v>43556</v>
       </c>
       <c r="G302" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7">
+      <c r="A303" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B303" t="s">
+        <v>31</v>
+      </c>
+      <c r="C303" s="1">
+        <v>1994</v>
+      </c>
+      <c r="D303">
+        <v>92</v>
+      </c>
+      <c r="E303">
+        <v>95</v>
+      </c>
+      <c r="F303" s="2">
+        <v>34790</v>
+      </c>
+      <c r="G303" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7">
+      <c r="A304" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B304" t="s">
+        <v>31</v>
+      </c>
+      <c r="C304" s="1">
+        <v>1995</v>
+      </c>
+      <c r="D304">
+        <v>94</v>
+      </c>
+      <c r="E304">
+        <v>96</v>
+      </c>
+      <c r="F304" s="2">
+        <v>35156</v>
+      </c>
+      <c r="G304" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7">
+      <c r="A305" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B305" t="s">
+        <v>31</v>
+      </c>
+      <c r="C305" s="1">
+        <v>1996</v>
+      </c>
+      <c r="D305">
+        <v>96</v>
+      </c>
+      <c r="E305">
+        <v>100</v>
+      </c>
+      <c r="F305" s="2">
+        <v>35521</v>
+      </c>
+      <c r="G305" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7">
+      <c r="A306" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B306" t="s">
+        <v>31</v>
+      </c>
+      <c r="C306" s="1">
+        <v>1997</v>
+      </c>
+      <c r="D306">
+        <v>91</v>
+      </c>
+      <c r="E306">
+        <v>93</v>
+      </c>
+      <c r="F306" s="2">
+        <v>35886</v>
+      </c>
+      <c r="G306" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7">
+      <c r="A307" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B307" t="s">
+        <v>31</v>
+      </c>
+      <c r="C307" s="1">
+        <v>1998</v>
+      </c>
+      <c r="D307">
+        <v>90</v>
+      </c>
+      <c r="E307">
+        <v>93</v>
+      </c>
+      <c r="F307" s="2">
+        <v>36251</v>
+      </c>
+      <c r="G307" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7">
+      <c r="A308" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B308" t="s">
+        <v>31</v>
+      </c>
+      <c r="C308" s="1">
+        <v>1999</v>
+      </c>
+      <c r="D308">
+        <v>90</v>
+      </c>
+      <c r="E308">
+        <v>92</v>
+      </c>
+      <c r="F308" s="2">
+        <v>36617</v>
+      </c>
+      <c r="G308" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7">
+      <c r="A309" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B309" t="s">
+        <v>31</v>
+      </c>
+      <c r="C309" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D309">
+        <v>94</v>
+      </c>
+      <c r="E309">
+        <v>96</v>
+      </c>
+      <c r="F309" s="2">
+        <v>36982</v>
+      </c>
+      <c r="G309" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7">
+      <c r="A310" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B310" t="s">
+        <v>31</v>
+      </c>
+      <c r="C310" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D310">
+        <v>91</v>
+      </c>
+      <c r="E310">
+        <v>93</v>
+      </c>
+      <c r="F310" s="2">
+        <v>37347</v>
+      </c>
+      <c r="G310" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7">
+      <c r="A311" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B311" t="s">
+        <v>31</v>
+      </c>
+      <c r="C311" s="1">
+        <v>2002</v>
+      </c>
+      <c r="D311">
+        <v>94</v>
+      </c>
+      <c r="E311">
+        <v>97</v>
+      </c>
+      <c r="F311" s="2">
+        <v>37895</v>
+      </c>
+      <c r="G311" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7">
+      <c r="A312" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B312" t="s">
+        <v>31</v>
+      </c>
+      <c r="C312" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D312">
+        <v>94</v>
+      </c>
+      <c r="E312">
+        <v>96</v>
+      </c>
+      <c r="F312" s="2">
+        <v>38078</v>
+      </c>
+      <c r="G312" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7">
+      <c r="A313" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B313" t="s">
+        <v>31</v>
+      </c>
+      <c r="C313" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D313">
+        <v>91</v>
+      </c>
+      <c r="E313">
+        <v>93</v>
+      </c>
+      <c r="F313" s="2">
+        <v>38443</v>
+      </c>
+      <c r="G313" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7">
+      <c r="A314" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B314" t="s">
+        <v>31</v>
+      </c>
+      <c r="C314" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D314">
+        <v>92</v>
+      </c>
+      <c r="E314">
+        <v>94</v>
+      </c>
+      <c r="F314" s="2">
+        <v>38808</v>
+      </c>
+      <c r="G314" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7">
+      <c r="A315" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B315" t="s">
+        <v>31</v>
+      </c>
+      <c r="C315" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D315">
+        <v>93</v>
+      </c>
+      <c r="E315">
+        <v>95</v>
+      </c>
+      <c r="F315" s="2">
+        <v>39173</v>
+      </c>
+      <c r="G315" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7">
+      <c r="A316" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B316" t="s">
+        <v>31</v>
+      </c>
+      <c r="C316" s="1">
+        <v>2007</v>
+      </c>
+      <c r="D316">
+        <v>92</v>
+      </c>
+      <c r="E316">
+        <v>95</v>
+      </c>
+      <c r="F316" s="2">
+        <v>39539</v>
+      </c>
+      <c r="G316" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7">
+      <c r="A317" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B317" t="s">
+        <v>31</v>
+      </c>
+      <c r="C317" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D317">
+        <v>95</v>
+      </c>
+      <c r="E317">
+        <v>97</v>
+      </c>
+      <c r="F317" s="2">
+        <v>39904</v>
+      </c>
+      <c r="G317" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7">
+      <c r="A318" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B318" t="s">
+        <v>31</v>
+      </c>
+      <c r="C318" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D318">
+        <v>96</v>
+      </c>
+      <c r="E318">
+        <v>100</v>
+      </c>
+      <c r="F318" s="2">
+        <v>40269</v>
+      </c>
+      <c r="G318" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7">
+      <c r="A319" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B319" t="s">
+        <v>31</v>
+      </c>
+      <c r="C319" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D319">
+        <v>95</v>
+      </c>
+      <c r="E319">
+        <v>98</v>
+      </c>
+      <c r="F319" s="2">
+        <v>40664</v>
+      </c>
+      <c r="G319" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7">
+      <c r="A320" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B320" t="s">
+        <v>31</v>
+      </c>
+      <c r="C320" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D320">
+        <v>93</v>
+      </c>
+      <c r="E320">
+        <v>95</v>
+      </c>
+      <c r="F320" s="2">
+        <v>41000</v>
+      </c>
+      <c r="G320" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7">
+      <c r="A321" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B321" t="s">
+        <v>31</v>
+      </c>
+      <c r="C321" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D321">
+        <v>93</v>
+      </c>
+      <c r="E321">
+        <v>95</v>
+      </c>
+      <c r="F321" s="2">
+        <v>41365</v>
+      </c>
+      <c r="G321" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7">
+      <c r="A322" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B322" t="s">
+        <v>31</v>
+      </c>
+      <c r="C322" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D322">
+        <v>89</v>
+      </c>
+      <c r="E322">
+        <v>92</v>
+      </c>
+      <c r="F322" s="2">
+        <v>41852</v>
+      </c>
+      <c r="G322" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7">
+      <c r="A323" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B323" t="s">
+        <v>31</v>
+      </c>
+      <c r="C323" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D323">
+        <v>94</v>
+      </c>
+      <c r="E323">
+        <v>96</v>
+      </c>
+      <c r="F323" s="2">
+        <v>42095</v>
+      </c>
+      <c r="G323" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7">
+      <c r="A324" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B324" t="s">
+        <v>31</v>
+      </c>
+      <c r="C324" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D324">
+        <v>95</v>
+      </c>
+      <c r="E324">
+        <v>97</v>
+      </c>
+      <c r="F324" s="2">
+        <v>42461</v>
+      </c>
+      <c r="G324" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7">
+      <c r="A325" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B325" t="s">
+        <v>31</v>
+      </c>
+      <c r="C325" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D325">
+        <v>98</v>
+      </c>
+      <c r="E325">
+        <v>100</v>
+      </c>
+      <c r="F325" s="2">
+        <v>42826</v>
+      </c>
+      <c r="G325" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7">
+      <c r="A326" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B326" t="s">
+        <v>31</v>
+      </c>
+      <c r="C326" s="1">
+        <v>2017</v>
+      </c>
+      <c r="D326">
+        <v>96</v>
+      </c>
+      <c r="E326">
+        <v>98</v>
+      </c>
+      <c r="F326" s="2">
+        <v>43191</v>
+      </c>
+      <c r="G326" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7">
+      <c r="A327" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B327" t="s">
+        <v>31</v>
+      </c>
+      <c r="C327" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D327">
+        <v>98</v>
+      </c>
+      <c r="E327">
+        <v>100</v>
+      </c>
+      <c r="F327" s="2">
+        <v>43556</v>
+      </c>
+      <c r="G327" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement separated weather sources.
</commit_message>
<xml_diff>
--- a/data/ratings.xlsx
+++ b/data/ratings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ML\WineML\GrandCruClassifier\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5638926-B2B4-4F60-95EB-FE585165D72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F845E69-7629-4F97-BADB-70B21A56CDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="2592" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First Rating" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="35">
   <si>
     <t>Vintage</t>
   </si>
@@ -97,22 +97,10 @@
     <t>Château Palmer</t>
   </si>
   <si>
-    <t>Château Lafite Rothschild Pauillac</t>
-  </si>
-  <si>
-    <t>Château Latour Pauillac</t>
-  </si>
-  <si>
     <t>Château Cheval Blanc</t>
   </si>
   <si>
-    <t>Petrus Pomerol</t>
-  </si>
-  <si>
     <t>Château Pavie</t>
-  </si>
-  <si>
-    <t>Château Léoville Las Cases Saint-Julien</t>
   </si>
   <si>
     <t>Pomerol</t>
@@ -124,7 +112,25 @@
     <t>Médoc</t>
   </si>
   <si>
-    <t>Château Pichon-Longueville Comtesse de Lalande Pauillac</t>
+    <t>Château Lafite Rothschild</t>
+  </si>
+  <si>
+    <t>Château Latour</t>
+  </si>
+  <si>
+    <t>Château Mouton Rothschild</t>
+  </si>
+  <si>
+    <t>Château Haut-Brion</t>
+  </si>
+  <si>
+    <t>Petrus</t>
+  </si>
+  <si>
+    <t>Château Léoville Las Cases</t>
+  </si>
+  <si>
+    <t>Château Pichon-Longueville Comtesse de Lalande</t>
   </si>
 </sst>
 </file>
@@ -463,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -501,10 +507,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1994</v>
@@ -524,10 +530,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
         <v>1995</v>
@@ -547,10 +553,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4">
         <v>1996</v>
@@ -570,10 +576,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>1997</v>
@@ -593,10 +599,10 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>1998</v>
@@ -616,10 +622,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
         <v>1999</v>
@@ -639,10 +645,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>2000</v>
@@ -662,10 +668,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1">
         <v>2001</v>
@@ -685,10 +691,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>2002</v>
@@ -708,10 +714,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1">
         <v>2003</v>
@@ -731,10 +737,10 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>2004</v>
@@ -754,10 +760,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1">
         <v>2005</v>
@@ -777,10 +783,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>2006</v>
@@ -800,10 +806,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1">
         <v>2007</v>
@@ -823,10 +829,10 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16">
         <v>2008</v>
@@ -846,10 +852,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1">
         <v>2009</v>
@@ -869,10 +875,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18">
         <v>2010</v>
@@ -892,10 +898,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1">
         <v>2011</v>
@@ -915,10 +921,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C20">
         <v>2012</v>
@@ -938,10 +944,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
         <v>2013</v>
@@ -961,10 +967,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>2014</v>
@@ -984,10 +990,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1">
         <v>2015</v>
@@ -1007,10 +1013,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>2016</v>
@@ -1030,10 +1036,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1">
         <v>2017</v>
@@ -1053,10 +1059,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>2018</v>
@@ -1076,10 +1082,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1">
         <v>1994</v>
@@ -1099,10 +1105,10 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>1995</v>
@@ -1122,10 +1128,10 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1">
         <v>1996</v>
@@ -1145,10 +1151,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <v>1997</v>
@@ -1168,10 +1174,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C31" s="1">
         <v>1998</v>
@@ -1191,10 +1197,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C32">
         <v>1999</v>
@@ -1214,10 +1220,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1">
         <v>2000</v>
@@ -1237,10 +1243,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C34">
         <v>2001</v>
@@ -1260,10 +1266,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C35" s="1">
         <v>2002</v>
@@ -1283,10 +1289,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C36">
         <v>2003</v>
@@ -1306,10 +1312,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C37" s="1">
         <v>2004</v>
@@ -1329,10 +1335,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C38">
         <v>2005</v>
@@ -1352,10 +1358,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1">
         <v>2006</v>
@@ -1375,10 +1381,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C40">
         <v>2007</v>
@@ -1398,10 +1404,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C41" s="1">
         <v>2008</v>
@@ -1421,10 +1427,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C42">
         <v>2009</v>
@@ -1444,10 +1450,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1">
         <v>2010</v>
@@ -1467,10 +1473,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C44">
         <v>2011</v>
@@ -1490,10 +1496,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C45" s="1">
         <v>2012</v>
@@ -1513,10 +1519,10 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C46">
         <v>2013</v>
@@ -1536,10 +1542,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C47" s="1">
         <v>2014</v>
@@ -1559,10 +1565,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C48">
         <v>2015</v>
@@ -1582,10 +1588,10 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C49" s="1">
         <v>2016</v>
@@ -1605,10 +1611,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C50">
         <v>2017</v>
@@ -1628,10 +1634,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C51" s="1">
         <v>2018</v>
@@ -1651,10 +1657,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C52">
         <v>1994</v>
@@ -1674,10 +1680,10 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C53" s="1">
         <v>1995</v>
@@ -1697,10 +1703,10 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C54">
         <v>1996</v>
@@ -1720,10 +1726,10 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C55" s="1">
         <v>1997</v>
@@ -1743,10 +1749,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C56">
         <v>1998</v>
@@ -1766,10 +1772,10 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C57" s="1">
         <v>1999</v>
@@ -1789,10 +1795,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C58">
         <v>2000</v>
@@ -1812,10 +1818,10 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C59" s="1">
         <v>2001</v>
@@ -1835,10 +1841,10 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C60">
         <v>2002</v>
@@ -1858,10 +1864,10 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C61" s="1">
         <v>2003</v>
@@ -1881,10 +1887,10 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C62">
         <v>2004</v>
@@ -1904,10 +1910,10 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C63" s="1">
         <v>2005</v>
@@ -1927,10 +1933,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C64">
         <v>2006</v>
@@ -1950,10 +1956,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C65" s="1">
         <v>2007</v>
@@ -1973,10 +1979,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C66">
         <v>2008</v>
@@ -1996,10 +2002,10 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C67" s="1">
         <v>2009</v>
@@ -2019,10 +2025,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C68">
         <v>2010</v>
@@ -2042,10 +2048,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C69" s="1">
         <v>2011</v>
@@ -2065,10 +2071,10 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C70">
         <v>2012</v>
@@ -2088,10 +2094,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C71" s="1">
         <v>2013</v>
@@ -2111,10 +2117,10 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C72">
         <v>2014</v>
@@ -2134,10 +2140,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C73" s="1">
         <v>2015</v>
@@ -2157,10 +2163,10 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C74">
         <v>2016</v>
@@ -2180,10 +2186,10 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C75" s="1">
         <v>2017</v>
@@ -2203,10 +2209,10 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="1" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C76">
         <v>2018</v>
@@ -2226,10 +2232,10 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B77" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C77" s="1">
         <v>1994</v>
@@ -2249,10 +2255,10 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B78" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C78">
         <v>1995</v>
@@ -2272,10 +2278,10 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C79" s="1">
         <v>1996</v>
@@ -2295,10 +2301,10 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B80" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C80">
         <v>1997</v>
@@ -2318,10 +2324,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C81" s="1">
         <v>1998</v>
@@ -2341,10 +2347,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C82">
         <v>1999</v>
@@ -2364,10 +2370,10 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B83" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C83" s="1">
         <v>2000</v>
@@ -2387,10 +2393,10 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B84" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C84">
         <v>2001</v>
@@ -2410,10 +2416,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C85" s="1">
         <v>2002</v>
@@ -2433,10 +2439,10 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B86" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C86">
         <v>2003</v>
@@ -2456,10 +2462,10 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B87" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C87" s="1">
         <v>2004</v>
@@ -2479,10 +2485,10 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C88">
         <v>2005</v>
@@ -2502,10 +2508,10 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C89" s="1">
         <v>2006</v>
@@ -2525,10 +2531,10 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B90" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C90">
         <v>2007</v>
@@ -2548,10 +2554,10 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C91" s="1">
         <v>2008</v>
@@ -2571,10 +2577,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B92" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C92">
         <v>2009</v>
@@ -2594,10 +2600,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B93" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C93" s="1">
         <v>2010</v>
@@ -2617,10 +2623,10 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B94" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C94">
         <v>2011</v>
@@ -2640,10 +2646,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B95" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C95" s="1">
         <v>2012</v>
@@ -2663,10 +2669,10 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B96" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C96">
         <v>2013</v>
@@ -2686,10 +2692,10 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B97" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C97" s="1">
         <v>2014</v>
@@ -2709,10 +2715,10 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C98">
         <v>2015</v>
@@ -2732,10 +2738,10 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B99" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C99" s="1">
         <v>2016</v>
@@ -2755,10 +2761,10 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B100" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C100">
         <v>2017</v>
@@ -2778,10 +2784,10 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C101" s="1">
         <v>2018</v>
@@ -2804,7 +2810,7 @@
         <v>6</v>
       </c>
       <c r="B102" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C102">
         <v>1994</v>
@@ -2827,7 +2833,7 @@
         <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C103" s="1">
         <v>1995</v>
@@ -2850,7 +2856,7 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C104">
         <v>1996</v>
@@ -2873,7 +2879,7 @@
         <v>6</v>
       </c>
       <c r="B105" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C105" s="1">
         <v>1997</v>
@@ -2896,7 +2902,7 @@
         <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C106">
         <v>1998</v>
@@ -2919,7 +2925,7 @@
         <v>6</v>
       </c>
       <c r="B107" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C107" s="1">
         <v>1999</v>
@@ -2942,7 +2948,7 @@
         <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C108">
         <v>2000</v>
@@ -2965,7 +2971,7 @@
         <v>6</v>
       </c>
       <c r="B109" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C109" s="1">
         <v>2001</v>
@@ -2988,7 +2994,7 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C110">
         <v>2002</v>
@@ -3011,7 +3017,7 @@
         <v>6</v>
       </c>
       <c r="B111" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C111" s="1">
         <v>2003</v>
@@ -3034,7 +3040,7 @@
         <v>6</v>
       </c>
       <c r="B112" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C112">
         <v>2004</v>
@@ -3057,7 +3063,7 @@
         <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C113" s="1">
         <v>2005</v>
@@ -3080,7 +3086,7 @@
         <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C114">
         <v>2006</v>
@@ -3103,7 +3109,7 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C115" s="1">
         <v>2007</v>
@@ -3126,7 +3132,7 @@
         <v>6</v>
       </c>
       <c r="B116" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C116">
         <v>2008</v>
@@ -3149,7 +3155,7 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C117" s="1">
         <v>2009</v>
@@ -3172,7 +3178,7 @@
         <v>6</v>
       </c>
       <c r="B118" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C118">
         <v>2010</v>
@@ -3195,7 +3201,7 @@
         <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C119" s="1">
         <v>2011</v>
@@ -3218,7 +3224,7 @@
         <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C120">
         <v>2012</v>
@@ -3241,7 +3247,7 @@
         <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C121" s="1">
         <v>2013</v>
@@ -3264,7 +3270,7 @@
         <v>6</v>
       </c>
       <c r="B122" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C122">
         <v>2014</v>
@@ -3287,7 +3293,7 @@
         <v>6</v>
       </c>
       <c r="B123" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C123" s="1">
         <v>2015</v>
@@ -3310,7 +3316,7 @@
         <v>6</v>
       </c>
       <c r="B124" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C124">
         <v>2016</v>
@@ -3333,7 +3339,7 @@
         <v>6</v>
       </c>
       <c r="B125" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C125" s="1">
         <v>2017</v>
@@ -3356,7 +3362,7 @@
         <v>6</v>
       </c>
       <c r="B126" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C126">
         <v>2018</v>
@@ -3379,7 +3385,7 @@
         <v>7</v>
       </c>
       <c r="B127" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C127" s="1">
         <v>1994</v>
@@ -3402,7 +3408,7 @@
         <v>7</v>
       </c>
       <c r="B128" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C128">
         <v>1995</v>
@@ -3425,7 +3431,7 @@
         <v>7</v>
       </c>
       <c r="B129" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C129" s="1">
         <v>1996</v>
@@ -3448,7 +3454,7 @@
         <v>7</v>
       </c>
       <c r="B130" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C130">
         <v>1997</v>
@@ -3471,7 +3477,7 @@
         <v>7</v>
       </c>
       <c r="B131" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C131" s="1">
         <v>1998</v>
@@ -3494,7 +3500,7 @@
         <v>7</v>
       </c>
       <c r="B132" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C132">
         <v>1999</v>
@@ -3517,7 +3523,7 @@
         <v>7</v>
       </c>
       <c r="B133" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C133" s="1">
         <v>2000</v>
@@ -3540,7 +3546,7 @@
         <v>7</v>
       </c>
       <c r="B134" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C134">
         <v>2001</v>
@@ -3563,7 +3569,7 @@
         <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C135" s="1">
         <v>2002</v>
@@ -3586,7 +3592,7 @@
         <v>7</v>
       </c>
       <c r="B136" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C136">
         <v>2003</v>
@@ -3609,7 +3615,7 @@
         <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C137" s="1">
         <v>2004</v>
@@ -3632,7 +3638,7 @@
         <v>7</v>
       </c>
       <c r="B138" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C138">
         <v>2005</v>
@@ -3655,7 +3661,7 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C139" s="1">
         <v>2006</v>
@@ -3678,7 +3684,7 @@
         <v>7</v>
       </c>
       <c r="B140" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C140">
         <v>2007</v>
@@ -3701,7 +3707,7 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C141" s="1">
         <v>2008</v>
@@ -3724,7 +3730,7 @@
         <v>7</v>
       </c>
       <c r="B142" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C142">
         <v>2009</v>
@@ -3747,7 +3753,7 @@
         <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C143" s="1">
         <v>2010</v>
@@ -3770,7 +3776,7 @@
         <v>7</v>
       </c>
       <c r="B144" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C144">
         <v>2011</v>
@@ -3793,7 +3799,7 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C145" s="1">
         <v>2012</v>
@@ -3816,7 +3822,7 @@
         <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C146">
         <v>2013</v>
@@ -3839,7 +3845,7 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C147" s="1">
         <v>2014</v>
@@ -3862,7 +3868,7 @@
         <v>7</v>
       </c>
       <c r="B148" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C148">
         <v>2015</v>
@@ -3885,7 +3891,7 @@
         <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C149" s="1">
         <v>2016</v>
@@ -3908,7 +3914,7 @@
         <v>7</v>
       </c>
       <c r="B150" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C150">
         <v>2017</v>
@@ -3931,7 +3937,7 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C151" s="1">
         <v>2018</v>
@@ -3951,10 +3957,10 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B152" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C152">
         <v>1994</v>
@@ -3974,10 +3980,10 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B153" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C153" s="1">
         <v>1995</v>
@@ -3997,10 +4003,10 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B154" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C154">
         <v>1996</v>
@@ -4020,10 +4026,10 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B155" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C155" s="1">
         <v>1997</v>
@@ -4043,10 +4049,10 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B156" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C156">
         <v>1998</v>
@@ -4066,10 +4072,10 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B157" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C157" s="1">
         <v>1999</v>
@@ -4089,10 +4095,10 @@
     </row>
     <row r="158" spans="1:7">
       <c r="A158" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B158" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C158">
         <v>2000</v>
@@ -4112,10 +4118,10 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B159" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C159" s="1">
         <v>2001</v>
@@ -4135,10 +4141,10 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B160" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C160">
         <v>2002</v>
@@ -4158,10 +4164,10 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B161" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C161" s="1">
         <v>2003</v>
@@ -4181,10 +4187,10 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B162" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C162">
         <v>2004</v>
@@ -4204,10 +4210,10 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B163" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C163" s="1">
         <v>2005</v>
@@ -4227,10 +4233,10 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B164" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C164">
         <v>2006</v>
@@ -4250,10 +4256,10 @@
     </row>
     <row r="165" spans="1:7">
       <c r="A165" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B165" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C165" s="1">
         <v>2007</v>
@@ -4273,10 +4279,10 @@
     </row>
     <row r="166" spans="1:7">
       <c r="A166" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B166" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C166">
         <v>2008</v>
@@ -4296,10 +4302,10 @@
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B167" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C167" s="1">
         <v>2009</v>
@@ -4319,10 +4325,10 @@
     </row>
     <row r="168" spans="1:7">
       <c r="A168" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B168" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C168">
         <v>2010</v>
@@ -4342,10 +4348,10 @@
     </row>
     <row r="169" spans="1:7">
       <c r="A169" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B169" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C169" s="1">
         <v>2011</v>
@@ -4365,10 +4371,10 @@
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B170" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C170">
         <v>2012</v>
@@ -4388,10 +4394,10 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B171" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C171" s="1">
         <v>2013</v>
@@ -4411,10 +4417,10 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B172" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C172">
         <v>2014</v>
@@ -4434,10 +4440,10 @@
     </row>
     <row r="173" spans="1:7">
       <c r="A173" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B173" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C173" s="1">
         <v>2015</v>
@@ -4457,10 +4463,10 @@
     </row>
     <row r="174" spans="1:7">
       <c r="A174" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B174" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C174">
         <v>2016</v>
@@ -4480,10 +4486,10 @@
     </row>
     <row r="175" spans="1:7">
       <c r="A175" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B175" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C175" s="1">
         <v>2017</v>
@@ -4503,10 +4509,10 @@
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B176" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C176">
         <v>2018</v>
@@ -4529,7 +4535,7 @@
         <v>21</v>
       </c>
       <c r="B177" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C177" s="1">
         <v>1994</v>
@@ -4552,7 +4558,7 @@
         <v>21</v>
       </c>
       <c r="B178" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C178" s="1">
         <v>1995</v>
@@ -4575,7 +4581,7 @@
         <v>21</v>
       </c>
       <c r="B179" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C179" s="1">
         <v>1996</v>
@@ -4598,7 +4604,7 @@
         <v>21</v>
       </c>
       <c r="B180" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C180" s="1">
         <v>1997</v>
@@ -4621,7 +4627,7 @@
         <v>21</v>
       </c>
       <c r="B181" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C181" s="1">
         <v>1998</v>
@@ -4644,7 +4650,7 @@
         <v>21</v>
       </c>
       <c r="B182" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C182" s="1">
         <v>1999</v>
@@ -4667,7 +4673,7 @@
         <v>21</v>
       </c>
       <c r="B183" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C183" s="1">
         <v>2000</v>
@@ -4690,7 +4696,7 @@
         <v>21</v>
       </c>
       <c r="B184" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C184" s="1">
         <v>2001</v>
@@ -4713,7 +4719,7 @@
         <v>21</v>
       </c>
       <c r="B185" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C185" s="1">
         <v>2002</v>
@@ -4736,7 +4742,7 @@
         <v>21</v>
       </c>
       <c r="B186" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C186" s="1">
         <v>2003</v>
@@ -4759,7 +4765,7 @@
         <v>21</v>
       </c>
       <c r="B187" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C187" s="1">
         <v>2004</v>
@@ -4782,7 +4788,7 @@
         <v>21</v>
       </c>
       <c r="B188" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C188" s="1">
         <v>2005</v>
@@ -4805,7 +4811,7 @@
         <v>21</v>
       </c>
       <c r="B189" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C189" s="1">
         <v>2006</v>
@@ -4828,7 +4834,7 @@
         <v>21</v>
       </c>
       <c r="B190" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C190" s="1">
         <v>2007</v>
@@ -4851,7 +4857,7 @@
         <v>21</v>
       </c>
       <c r="B191" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C191" s="1">
         <v>2008</v>
@@ -4874,7 +4880,7 @@
         <v>21</v>
       </c>
       <c r="B192" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C192" s="1">
         <v>2009</v>
@@ -4897,7 +4903,7 @@
         <v>21</v>
       </c>
       <c r="B193" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C193" s="1">
         <v>2010</v>
@@ -4920,7 +4926,7 @@
         <v>21</v>
       </c>
       <c r="B194" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C194" s="1">
         <v>2011</v>
@@ -4943,7 +4949,7 @@
         <v>21</v>
       </c>
       <c r="B195" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C195" s="1">
         <v>2012</v>
@@ -4966,7 +4972,7 @@
         <v>21</v>
       </c>
       <c r="B196" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C196" s="1">
         <v>2013</v>
@@ -4989,7 +4995,7 @@
         <v>21</v>
       </c>
       <c r="B197" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C197" s="1">
         <v>2014</v>
@@ -5012,7 +5018,7 @@
         <v>21</v>
       </c>
       <c r="B198" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C198" s="1">
         <v>2015</v>
@@ -5035,7 +5041,7 @@
         <v>21</v>
       </c>
       <c r="B199" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C199" s="1">
         <v>2016</v>
@@ -5058,7 +5064,7 @@
         <v>21</v>
       </c>
       <c r="B200" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C200" s="1">
         <v>2017</v>
@@ -5081,7 +5087,7 @@
         <v>21</v>
       </c>
       <c r="B201" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C201" s="1">
         <v>2018</v>
@@ -5104,7 +5110,7 @@
         <v>20</v>
       </c>
       <c r="B202" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C202" s="1">
         <v>1994</v>
@@ -5127,7 +5133,7 @@
         <v>20</v>
       </c>
       <c r="B203" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C203" s="1">
         <v>1995</v>
@@ -5150,7 +5156,7 @@
         <v>20</v>
       </c>
       <c r="B204" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C204" s="1">
         <v>1996</v>
@@ -5173,7 +5179,7 @@
         <v>20</v>
       </c>
       <c r="B205" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C205" s="1">
         <v>1997</v>
@@ -5196,7 +5202,7 @@
         <v>20</v>
       </c>
       <c r="B206" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C206" s="1">
         <v>1998</v>
@@ -5219,7 +5225,7 @@
         <v>20</v>
       </c>
       <c r="B207" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C207" s="1">
         <v>1999</v>
@@ -5242,7 +5248,7 @@
         <v>20</v>
       </c>
       <c r="B208" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C208" s="1">
         <v>2000</v>
@@ -5265,7 +5271,7 @@
         <v>20</v>
       </c>
       <c r="B209" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C209" s="1">
         <v>2001</v>
@@ -5288,7 +5294,7 @@
         <v>20</v>
       </c>
       <c r="B210" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C210" s="1">
         <v>2002</v>
@@ -5311,7 +5317,7 @@
         <v>20</v>
       </c>
       <c r="B211" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C211" s="1">
         <v>2003</v>
@@ -5334,7 +5340,7 @@
         <v>20</v>
       </c>
       <c r="B212" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C212" s="1">
         <v>2004</v>
@@ -5357,7 +5363,7 @@
         <v>20</v>
       </c>
       <c r="B213" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C213" s="1">
         <v>2005</v>
@@ -5380,7 +5386,7 @@
         <v>20</v>
       </c>
       <c r="B214" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C214" s="1">
         <v>2006</v>
@@ -5403,7 +5409,7 @@
         <v>20</v>
       </c>
       <c r="B215" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C215" s="1">
         <v>2007</v>
@@ -5426,7 +5432,7 @@
         <v>20</v>
       </c>
       <c r="B216" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C216" s="1">
         <v>2008</v>
@@ -5449,7 +5455,7 @@
         <v>20</v>
       </c>
       <c r="B217" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C217" s="1">
         <v>2009</v>
@@ -5472,7 +5478,7 @@
         <v>20</v>
       </c>
       <c r="B218" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C218" s="1">
         <v>2010</v>
@@ -5495,7 +5501,7 @@
         <v>20</v>
       </c>
       <c r="B219" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C219" s="1">
         <v>2011</v>
@@ -5518,7 +5524,7 @@
         <v>20</v>
       </c>
       <c r="B220" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C220" s="1">
         <v>2012</v>
@@ -5541,7 +5547,7 @@
         <v>20</v>
       </c>
       <c r="B221" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C221" s="1">
         <v>2013</v>
@@ -5564,7 +5570,7 @@
         <v>20</v>
       </c>
       <c r="B222" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C222" s="1">
         <v>2014</v>
@@ -5587,7 +5593,7 @@
         <v>20</v>
       </c>
       <c r="B223" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C223" s="1">
         <v>2015</v>
@@ -5610,7 +5616,7 @@
         <v>20</v>
       </c>
       <c r="B224" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C224" s="1">
         <v>2016</v>
@@ -5633,7 +5639,7 @@
         <v>20</v>
       </c>
       <c r="B225" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C225" s="1">
         <v>2017</v>
@@ -5656,7 +5662,7 @@
         <v>20</v>
       </c>
       <c r="B226" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C226" s="1">
         <v>2018</v>
@@ -5679,7 +5685,7 @@
         <v>22</v>
       </c>
       <c r="B227" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C227" s="1">
         <v>1994</v>
@@ -5702,7 +5708,7 @@
         <v>22</v>
       </c>
       <c r="B228" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C228" s="1">
         <v>1995</v>
@@ -5725,7 +5731,7 @@
         <v>22</v>
       </c>
       <c r="B229" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C229" s="1">
         <v>1996</v>
@@ -5748,7 +5754,7 @@
         <v>22</v>
       </c>
       <c r="B230" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C230" s="1">
         <v>1997</v>
@@ -5771,7 +5777,7 @@
         <v>22</v>
       </c>
       <c r="B231" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C231" s="1">
         <v>1998</v>
@@ -5794,7 +5800,7 @@
         <v>22</v>
       </c>
       <c r="B232" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C232" s="1">
         <v>1999</v>
@@ -5817,7 +5823,7 @@
         <v>22</v>
       </c>
       <c r="B233" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C233" s="1">
         <v>2000</v>
@@ -5840,7 +5846,7 @@
         <v>22</v>
       </c>
       <c r="B234" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C234" s="1">
         <v>2001</v>
@@ -5863,7 +5869,7 @@
         <v>22</v>
       </c>
       <c r="B235" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C235" s="1">
         <v>2002</v>
@@ -5886,7 +5892,7 @@
         <v>22</v>
       </c>
       <c r="B236" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C236" s="1">
         <v>2003</v>
@@ -5909,7 +5915,7 @@
         <v>22</v>
       </c>
       <c r="B237" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C237" s="1">
         <v>2004</v>
@@ -5932,7 +5938,7 @@
         <v>22</v>
       </c>
       <c r="B238" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C238" s="1">
         <v>2005</v>
@@ -5955,7 +5961,7 @@
         <v>22</v>
       </c>
       <c r="B239" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C239" s="1">
         <v>2006</v>
@@ -5978,7 +5984,7 @@
         <v>22</v>
       </c>
       <c r="B240" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C240" s="1">
         <v>2007</v>
@@ -6001,7 +6007,7 @@
         <v>22</v>
       </c>
       <c r="B241" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C241" s="1">
         <v>2008</v>
@@ -6024,7 +6030,7 @@
         <v>22</v>
       </c>
       <c r="B242" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C242" s="1">
         <v>2009</v>
@@ -6047,7 +6053,7 @@
         <v>22</v>
       </c>
       <c r="B243" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C243" s="1">
         <v>2010</v>
@@ -6070,7 +6076,7 @@
         <v>22</v>
       </c>
       <c r="B244" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C244" s="1">
         <v>2011</v>
@@ -6093,7 +6099,7 @@
         <v>22</v>
       </c>
       <c r="B245" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C245" s="1">
         <v>2012</v>
@@ -6116,7 +6122,7 @@
         <v>22</v>
       </c>
       <c r="B246" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C246" s="1">
         <v>2013</v>
@@ -6139,7 +6145,7 @@
         <v>22</v>
       </c>
       <c r="B247" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C247" s="1">
         <v>2014</v>
@@ -6162,7 +6168,7 @@
         <v>22</v>
       </c>
       <c r="B248" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C248" s="1">
         <v>2015</v>
@@ -6185,7 +6191,7 @@
         <v>22</v>
       </c>
       <c r="B249" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C249" s="1">
         <v>2016</v>
@@ -6208,7 +6214,7 @@
         <v>22</v>
       </c>
       <c r="B250" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C250" s="1">
         <v>2017</v>
@@ -6231,7 +6237,7 @@
         <v>22</v>
       </c>
       <c r="B251" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C251" s="1">
         <v>2018</v>
@@ -6251,10 +6257,10 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B252" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C252" s="1">
         <v>1994</v>
@@ -6274,10 +6280,10 @@
     </row>
     <row r="253" spans="1:7">
       <c r="A253" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B253" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C253" s="1">
         <v>1995</v>
@@ -6297,10 +6303,10 @@
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B254" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C254" s="1">
         <v>1996</v>
@@ -6320,10 +6326,10 @@
     </row>
     <row r="255" spans="1:7">
       <c r="A255" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B255" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C255" s="1">
         <v>1997</v>
@@ -6343,10 +6349,10 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B256" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C256" s="1">
         <v>1998</v>
@@ -6366,10 +6372,10 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B257" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C257" s="1">
         <v>1999</v>
@@ -6389,10 +6395,10 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B258" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C258" s="1">
         <v>2000</v>
@@ -6412,10 +6418,10 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B259" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C259" s="1">
         <v>2001</v>
@@ -6435,10 +6441,10 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B260" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C260" s="1">
         <v>2002</v>
@@ -6458,10 +6464,10 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B261" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C261" s="1">
         <v>2003</v>
@@ -6481,10 +6487,10 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B262" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C262" s="1">
         <v>2004</v>
@@ -6504,10 +6510,10 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B263" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C263" s="1">
         <v>2005</v>
@@ -6527,10 +6533,10 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B264" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C264" s="1">
         <v>2006</v>
@@ -6550,10 +6556,10 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B265" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C265" s="1">
         <v>2007</v>
@@ -6573,10 +6579,10 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B266" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C266" s="1">
         <v>2008</v>
@@ -6596,10 +6602,10 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B267" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C267" s="1">
         <v>2009</v>
@@ -6619,10 +6625,10 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B268" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C268" s="1">
         <v>2010</v>
@@ -6642,10 +6648,10 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B269" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C269" s="1">
         <v>2011</v>
@@ -6665,10 +6671,10 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B270" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C270" s="1">
         <v>2012</v>
@@ -6688,10 +6694,10 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B271" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C271" s="1">
         <v>2013</v>
@@ -6711,10 +6717,10 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B272" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C272" s="1">
         <v>2014</v>
@@ -6734,10 +6740,10 @@
     </row>
     <row r="273" spans="1:7">
       <c r="A273" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B273" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C273" s="1">
         <v>2015</v>
@@ -6757,10 +6763,10 @@
     </row>
     <row r="274" spans="1:7">
       <c r="A274" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B274" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C274" s="1">
         <v>2016</v>
@@ -6780,10 +6786,10 @@
     </row>
     <row r="275" spans="1:7">
       <c r="A275" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B275" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C275" s="1">
         <v>2017</v>
@@ -6803,10 +6809,10 @@
     </row>
     <row r="276" spans="1:7">
       <c r="A276" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B276" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C276" s="1">
         <v>2018</v>
@@ -6826,10 +6832,10 @@
     </row>
     <row r="277" spans="1:7">
       <c r="A277" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B277" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C277" s="1">
         <v>1994</v>
@@ -6849,10 +6855,10 @@
     </row>
     <row r="278" spans="1:7">
       <c r="A278" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B278" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C278" s="1">
         <v>1995</v>
@@ -6872,10 +6878,10 @@
     </row>
     <row r="279" spans="1:7">
       <c r="A279" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B279" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C279" s="1">
         <v>1996</v>
@@ -6895,10 +6901,10 @@
     </row>
     <row r="280" spans="1:7">
       <c r="A280" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B280" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C280" s="1">
         <v>1997</v>
@@ -6918,10 +6924,10 @@
     </row>
     <row r="281" spans="1:7">
       <c r="A281" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B281" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C281" s="1">
         <v>1998</v>
@@ -6941,10 +6947,10 @@
     </row>
     <row r="282" spans="1:7">
       <c r="A282" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B282" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C282" s="1">
         <v>1999</v>
@@ -6964,10 +6970,10 @@
     </row>
     <row r="283" spans="1:7">
       <c r="A283" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B283" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C283" s="1">
         <v>2000</v>
@@ -6987,10 +6993,10 @@
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B284" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C284" s="1">
         <v>2001</v>
@@ -7010,10 +7016,10 @@
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B285" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C285" s="1">
         <v>2002</v>
@@ -7033,10 +7039,10 @@
     </row>
     <row r="286" spans="1:7">
       <c r="A286" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B286" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C286" s="1">
         <v>2003</v>
@@ -7056,10 +7062,10 @@
     </row>
     <row r="287" spans="1:7">
       <c r="A287" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B287" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C287" s="1">
         <v>2004</v>
@@ -7079,10 +7085,10 @@
     </row>
     <row r="288" spans="1:7">
       <c r="A288" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B288" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C288" s="1">
         <v>2005</v>
@@ -7102,10 +7108,10 @@
     </row>
     <row r="289" spans="1:7">
       <c r="A289" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B289" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C289" s="1">
         <v>2006</v>
@@ -7125,10 +7131,10 @@
     </row>
     <row r="290" spans="1:7">
       <c r="A290" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B290" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C290" s="1">
         <v>2007</v>
@@ -7148,10 +7154,10 @@
     </row>
     <row r="291" spans="1:7">
       <c r="A291" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B291" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C291" s="1">
         <v>2008</v>
@@ -7171,10 +7177,10 @@
     </row>
     <row r="292" spans="1:7">
       <c r="A292" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B292" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C292" s="1">
         <v>2009</v>
@@ -7194,10 +7200,10 @@
     </row>
     <row r="293" spans="1:7">
       <c r="A293" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B293" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C293" s="1">
         <v>2010</v>
@@ -7217,10 +7223,10 @@
     </row>
     <row r="294" spans="1:7">
       <c r="A294" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B294" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C294" s="1">
         <v>2011</v>
@@ -7240,10 +7246,10 @@
     </row>
     <row r="295" spans="1:7">
       <c r="A295" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B295" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C295" s="1">
         <v>2012</v>
@@ -7263,10 +7269,10 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B296" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C296" s="1">
         <v>2013</v>
@@ -7286,10 +7292,10 @@
     </row>
     <row r="297" spans="1:7">
       <c r="A297" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B297" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C297" s="1">
         <v>2014</v>
@@ -7309,10 +7315,10 @@
     </row>
     <row r="298" spans="1:7">
       <c r="A298" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B298" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C298" s="1">
         <v>2015</v>
@@ -7332,10 +7338,10 @@
     </row>
     <row r="299" spans="1:7">
       <c r="A299" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B299" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C299" s="1">
         <v>2016</v>
@@ -7355,10 +7361,10 @@
     </row>
     <row r="300" spans="1:7">
       <c r="A300" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B300" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C300" s="1">
         <v>2017</v>
@@ -7378,10 +7384,10 @@
     </row>
     <row r="301" spans="1:7">
       <c r="A301" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B301" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C301" s="1">
         <v>2018</v>
@@ -7401,10 +7407,10 @@
     </row>
     <row r="302" spans="1:7">
       <c r="A302" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B302" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C302" s="1">
         <v>1994</v>
@@ -7424,10 +7430,10 @@
     </row>
     <row r="303" spans="1:7">
       <c r="A303" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B303" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C303" s="1">
         <v>1995</v>
@@ -7447,10 +7453,10 @@
     </row>
     <row r="304" spans="1:7">
       <c r="A304" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B304" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C304" s="1">
         <v>1996</v>
@@ -7470,10 +7476,10 @@
     </row>
     <row r="305" spans="1:7">
       <c r="A305" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B305" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C305" s="1">
         <v>1997</v>
@@ -7493,10 +7499,10 @@
     </row>
     <row r="306" spans="1:7">
       <c r="A306" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B306" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C306" s="1">
         <v>1998</v>
@@ -7516,10 +7522,10 @@
     </row>
     <row r="307" spans="1:7">
       <c r="A307" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B307" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C307" s="1">
         <v>1999</v>
@@ -7539,10 +7545,10 @@
     </row>
     <row r="308" spans="1:7">
       <c r="A308" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B308" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C308" s="1">
         <v>2000</v>
@@ -7562,10 +7568,10 @@
     </row>
     <row r="309" spans="1:7">
       <c r="A309" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B309" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C309" s="1">
         <v>2001</v>
@@ -7585,10 +7591,10 @@
     </row>
     <row r="310" spans="1:7">
       <c r="A310" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B310" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C310" s="1">
         <v>2002</v>
@@ -7608,10 +7614,10 @@
     </row>
     <row r="311" spans="1:7">
       <c r="A311" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B311" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C311" s="1">
         <v>2003</v>
@@ -7631,10 +7637,10 @@
     </row>
     <row r="312" spans="1:7">
       <c r="A312" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B312" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C312" s="1">
         <v>2004</v>
@@ -7654,10 +7660,10 @@
     </row>
     <row r="313" spans="1:7">
       <c r="A313" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B313" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C313" s="1">
         <v>2005</v>
@@ -7677,10 +7683,10 @@
     </row>
     <row r="314" spans="1:7">
       <c r="A314" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B314" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C314" s="1">
         <v>2006</v>
@@ -7700,10 +7706,10 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B315" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C315" s="1">
         <v>2007</v>
@@ -7723,10 +7729,10 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B316" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C316" s="1">
         <v>2008</v>
@@ -7746,10 +7752,10 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B317" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C317" s="1">
         <v>2009</v>
@@ -7769,10 +7775,10 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B318" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C318" s="1">
         <v>2010</v>
@@ -7792,10 +7798,10 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B319" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C319" s="1">
         <v>2011</v>
@@ -7815,10 +7821,10 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B320" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C320" s="1">
         <v>2012</v>
@@ -7838,10 +7844,10 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B321" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C321" s="1">
         <v>2013</v>
@@ -7861,10 +7867,10 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B322" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C322" s="1">
         <v>2014</v>
@@ -7884,10 +7890,10 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B323" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C323" s="1">
         <v>2015</v>
@@ -7907,10 +7913,10 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B324" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C324" s="1">
         <v>2016</v>
@@ -7930,10 +7936,10 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B325" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C325" s="1">
         <v>2017</v>
@@ -7953,10 +7959,10 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B326" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C326" s="1">
         <v>2018</v>
@@ -7976,10 +7982,10 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B327" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C327" s="1">
         <v>1994</v>
@@ -7999,10 +8005,10 @@
     </row>
     <row r="328" spans="1:7">
       <c r="A328" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B328" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C328" s="1">
         <v>1995</v>
@@ -8022,10 +8028,10 @@
     </row>
     <row r="329" spans="1:7">
       <c r="A329" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B329" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C329" s="1">
         <v>1996</v>
@@ -8045,10 +8051,10 @@
     </row>
     <row r="330" spans="1:7">
       <c r="A330" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B330" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C330" s="1">
         <v>1997</v>
@@ -8068,10 +8074,10 @@
     </row>
     <row r="331" spans="1:7">
       <c r="A331" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B331" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C331" s="1">
         <v>1998</v>
@@ -8091,10 +8097,10 @@
     </row>
     <row r="332" spans="1:7">
       <c r="A332" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B332" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C332" s="1">
         <v>1999</v>
@@ -8114,10 +8120,10 @@
     </row>
     <row r="333" spans="1:7">
       <c r="A333" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B333" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C333" s="1">
         <v>2000</v>
@@ -8137,10 +8143,10 @@
     </row>
     <row r="334" spans="1:7">
       <c r="A334" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B334" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C334" s="1">
         <v>2001</v>
@@ -8160,10 +8166,10 @@
     </row>
     <row r="335" spans="1:7">
       <c r="A335" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B335" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C335" s="1">
         <v>2002</v>
@@ -8183,10 +8189,10 @@
     </row>
     <row r="336" spans="1:7">
       <c r="A336" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B336" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C336" s="1">
         <v>2003</v>
@@ -8206,10 +8212,10 @@
     </row>
     <row r="337" spans="1:7">
       <c r="A337" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B337" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C337" s="1">
         <v>2004</v>
@@ -8229,10 +8235,10 @@
     </row>
     <row r="338" spans="1:7">
       <c r="A338" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B338" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C338" s="1">
         <v>2005</v>
@@ -8252,10 +8258,10 @@
     </row>
     <row r="339" spans="1:7">
       <c r="A339" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B339" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C339" s="1">
         <v>2006</v>
@@ -8275,10 +8281,10 @@
     </row>
     <row r="340" spans="1:7">
       <c r="A340" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B340" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C340" s="1">
         <v>2007</v>
@@ -8298,10 +8304,10 @@
     </row>
     <row r="341" spans="1:7">
       <c r="A341" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B341" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C341" s="1">
         <v>2008</v>
@@ -8321,10 +8327,10 @@
     </row>
     <row r="342" spans="1:7">
       <c r="A342" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B342" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C342" s="1">
         <v>2009</v>
@@ -8344,10 +8350,10 @@
     </row>
     <row r="343" spans="1:7">
       <c r="A343" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B343" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C343" s="1">
         <v>2010</v>
@@ -8367,10 +8373,10 @@
     </row>
     <row r="344" spans="1:7">
       <c r="A344" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B344" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C344" s="1">
         <v>2011</v>
@@ -8390,10 +8396,10 @@
     </row>
     <row r="345" spans="1:7">
       <c r="A345" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B345" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C345" s="1">
         <v>2012</v>
@@ -8413,10 +8419,10 @@
     </row>
     <row r="346" spans="1:7">
       <c r="A346" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B346" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C346" s="1">
         <v>2013</v>
@@ -8436,10 +8442,10 @@
     </row>
     <row r="347" spans="1:7">
       <c r="A347" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B347" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C347" s="1">
         <v>2014</v>
@@ -8459,10 +8465,10 @@
     </row>
     <row r="348" spans="1:7">
       <c r="A348" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B348" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C348" s="1">
         <v>2015</v>
@@ -8482,10 +8488,10 @@
     </row>
     <row r="349" spans="1:7">
       <c r="A349" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B349" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C349" s="1">
         <v>2016</v>
@@ -8505,10 +8511,10 @@
     </row>
     <row r="350" spans="1:7">
       <c r="A350" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B350" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C350" s="1">
         <v>2017</v>
@@ -8528,10 +8534,10 @@
     </row>
     <row r="351" spans="1:7">
       <c r="A351" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B351" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C351" s="1">
         <v>2018</v>

</xml_diff>